<commit_message>
more shin megami tensei
</commit_message>
<xml_diff>
--- a/shin-megami-tensei/checklist.xlsx
+++ b/shin-megami-tensei/checklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clark/Local/src/weatherspud/japanese-collectors-list/shin-megami-tensei/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FB865B9-0C14-724F-BA17-F81219150F61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{42C773ED-4BC1-BF42-9579-7824E75F69F6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="26880" windowHeight="16340" xr2:uid="{D4FC0F6A-6FE0-CD4C-A4BA-779FF194BB2D}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="73">
   <si>
     <t>year</t>
   </si>
@@ -159,6 +159,99 @@
   </si>
   <si>
     <t>Business Hall: Shin Megami Tensei RPG Awakening Edition Supplement</t>
+  </si>
+  <si>
+    <t>真・女神転生3‐NOCTURNE TRPG 東京受胎</t>
+  </si>
+  <si>
+    <t>Shin Megami Tensei 3-NOCTURNE TRPG Tokyo conception</t>
+  </si>
+  <si>
+    <t>Jive</t>
+  </si>
+  <si>
+    <t>nocturne-rulebook.jpg</t>
+  </si>
+  <si>
+    <t>nocturne-supplement.jpg</t>
+  </si>
+  <si>
+    <t>アマラ深界 真・女神転生3‐NOCTURNE TRPGサプリメント</t>
+  </si>
+  <si>
+    <t>Amara Deep World: Shin Megami Tensei 3-NOCTURNE TRPG Supplement</t>
+  </si>
+  <si>
+    <t>再会―See you again next world 真・女神転生3 NOCTURNE TRPGリプレイ</t>
+  </si>
+  <si>
+    <t>Reunion―See you again next world: Shin Megami Tensei 3 NOCTURNE TRPG Replay</t>
+  </si>
+  <si>
+    <t>nocturne-replay.jpg</t>
+  </si>
+  <si>
+    <t>真・女神転生TRPG　魔都東京200X</t>
+  </si>
+  <si>
+    <t>Shin Megami Tensei TRPG Magic City Tokyo 200X</t>
+  </si>
+  <si>
+    <t>200x-rulebook.jpg</t>
+  </si>
+  <si>
+    <t>金剛神界 真・女神転生TRPG魔都東京200Xサプリメント</t>
+  </si>
+  <si>
+    <t>200x-magic-city-tokyo.jpg</t>
+  </si>
+  <si>
+    <t>Kongo Shinkai: Shin Megami Tensei TRPG Magic City Tokyo 200X Supplement</t>
+  </si>
+  <si>
+    <t>TOKYOミレニアム 真・女神転生TRPG魔都東京200Xサプリメント</t>
+  </si>
+  <si>
+    <t>200x-tokyo-millenium.jpg</t>
+  </si>
+  <si>
+    <t>Tokyo Millennium: Shin Megami Tensei TRPG Magic City Tokyo 200X Supplement</t>
+  </si>
+  <si>
+    <t>セフィロトの魔界 真・女神転生TRPG魔都東京200Xサプリメント</t>
+  </si>
+  <si>
+    <t>Sephiroto's Makai: Shin Megami Tensei TRPG Magic City Tokyo 200X Supplement</t>
+  </si>
+  <si>
+    <t>200x-sephirots-hell.jpg</t>
+  </si>
+  <si>
+    <t>闇のプロファイル 真・女神転生TRPG魔都東京200X</t>
+  </si>
+  <si>
+    <t>200x-dark-profile.jpg</t>
+  </si>
+  <si>
+    <t>Profile of Darkness Shin Megami Tensei TRPG Magic City Tokyo 200X</t>
+  </si>
+  <si>
+    <t>異形科学 －ストレンジ・サイエンス 真・女神転生TRPG 魔都東京200X</t>
+  </si>
+  <si>
+    <t>Variant Science-Strange Science Shin Megami Tensei TRPG Magic City Tokyo 200X</t>
+  </si>
+  <si>
+    <t>200x-ragnarok.jpg</t>
+  </si>
+  <si>
+    <t>ラグナロク 真・女神転生TRPG魔都東京200X</t>
+  </si>
+  <si>
+    <t>Ragnarok: Shin Megami Tensei TRPG Magic City Tokyo 200X</t>
+  </si>
+  <si>
+    <t>200x-variant-science.jpg</t>
   </si>
 </sst>
 </file>
@@ -519,16 +612,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43E819AE-E18D-4044-98EA-EF00A692D0DF}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="57.6640625" customWidth="1"/>
-    <col min="3" max="3" width="56.5" customWidth="1"/>
+    <col min="2" max="2" width="66.83203125" customWidth="1"/>
+    <col min="3" max="3" width="73.83203125" customWidth="1"/>
     <col min="4" max="4" width="21.83203125" customWidth="1"/>
     <col min="5" max="5" width="58" customWidth="1"/>
   </cols>
@@ -753,6 +846,206 @@
         <v>17</v>
       </c>
     </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>2004</v>
+      </c>
+      <c r="B12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>2004</v>
+      </c>
+      <c r="B13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>2005</v>
+      </c>
+      <c r="B14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" t="s">
+        <v>51</v>
+      </c>
+      <c r="F14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>2005</v>
+      </c>
+      <c r="B15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" t="s">
+        <v>54</v>
+      </c>
+      <c r="F15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>2006</v>
+      </c>
+      <c r="B16" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" t="s">
+        <v>44</v>
+      </c>
+      <c r="E16" t="s">
+        <v>56</v>
+      </c>
+      <c r="F16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>2006</v>
+      </c>
+      <c r="B17" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" t="s">
+        <v>60</v>
+      </c>
+      <c r="D17" t="s">
+        <v>44</v>
+      </c>
+      <c r="E17" t="s">
+        <v>59</v>
+      </c>
+      <c r="F17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>2007</v>
+      </c>
+      <c r="B18" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" t="s">
+        <v>62</v>
+      </c>
+      <c r="D18" t="s">
+        <v>44</v>
+      </c>
+      <c r="E18" t="s">
+        <v>63</v>
+      </c>
+      <c r="F18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>2007</v>
+      </c>
+      <c r="B19" t="s">
+        <v>64</v>
+      </c>
+      <c r="C19" t="s">
+        <v>66</v>
+      </c>
+      <c r="D19" t="s">
+        <v>44</v>
+      </c>
+      <c r="E19" t="s">
+        <v>65</v>
+      </c>
+      <c r="F19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>2008</v>
+      </c>
+      <c r="B20" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" t="s">
+        <v>71</v>
+      </c>
+      <c r="D20" t="s">
+        <v>44</v>
+      </c>
+      <c r="E20" t="s">
+        <v>69</v>
+      </c>
+      <c r="F20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>2010</v>
+      </c>
+      <c r="B21" t="s">
+        <v>67</v>
+      </c>
+      <c r="C21" t="s">
+        <v>68</v>
+      </c>
+      <c r="D21" t="s">
+        <v>44</v>
+      </c>
+      <c r="E21" t="s">
+        <v>72</v>
+      </c>
+      <c r="F21" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>